<commit_message>
add 2 data paths
</commit_message>
<xml_diff>
--- a/example_hrd.xlsx
+++ b/example_hrd.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4137" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4137" uniqueCount="1088">
   <si>
     <t xml:space="preserve">E-Nummer</t>
   </si>
@@ -3276,6 +3276,12 @@
   </si>
   <si>
     <t xml:space="preserve">nur partielle Analyse:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/test/one/data/one.svs;/test/two/data/two.svs;/home/simon/philipp/pat_62/BRACS_1602/data/BRACS_1602.svs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/test/one/data/one.svs;/home/simon/philipp/pat_62/BRACS_1598/data/BRACS_1598.svs;/test/three/data/three.svs</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
@@ -3558,7 +3564,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="J1" activeCellId="1" sqref="AC49 J1"/>
+      <selection pane="bottomLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32680,8 +32686,8 @@
   </sheetPr>
   <dimension ref="A1:AE481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC49" activeCellId="0" sqref="AC49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33122,7 +33128,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>1075</v>
+        <v>1085</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0</v>
@@ -33980,7 +33986,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>1075</v>
+        <v>1086</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>0</v>
@@ -43251,7 +43257,7 @@
         <v>0</v>
       </c>
       <c r="H429" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I429" s="0" t="n">
         <v>1</v>
@@ -43268,7 +43274,7 @@
         <v>0</v>
       </c>
       <c r="H430" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I430" s="0" t="n">
         <v>1</v>
@@ -43288,7 +43294,7 @@
         <v>0</v>
       </c>
       <c r="H431" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I431" s="0" t="n">
         <v>1</v>
@@ -43305,7 +43311,7 @@
         <v>0</v>
       </c>
       <c r="H432" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I432" s="0" t="n">
         <v>1</v>
@@ -43322,7 +43328,7 @@
         <v>0</v>
       </c>
       <c r="H433" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I433" s="0" t="n">
         <v>1</v>
@@ -43342,7 +43348,7 @@
         <v>0</v>
       </c>
       <c r="H434" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I434" s="0" t="n">
         <v>1</v>
@@ -43359,7 +43365,7 @@
         <v>0</v>
       </c>
       <c r="H435" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I435" s="0" t="n">
         <v>1</v>
@@ -43376,7 +43382,7 @@
         <v>0</v>
       </c>
       <c r="H436" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I436" s="0" t="n">
         <v>1</v>
@@ -43393,10 +43399,10 @@
         <v>0</v>
       </c>
       <c r="H437" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I437" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J437" s="0" t="n">
         <v>0</v>
@@ -43416,10 +43422,10 @@
         <v>0</v>
       </c>
       <c r="H438" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I438" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J438" s="0" t="n">
         <v>0</v>
@@ -43436,10 +43442,10 @@
         <v>0</v>
       </c>
       <c r="H439" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I439" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J439" s="0" t="n">
         <v>0</v>
@@ -43456,10 +43462,10 @@
         <v>0</v>
       </c>
       <c r="H440" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I440" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J440" s="0" t="n">
         <v>0</v>
@@ -43476,10 +43482,10 @@
         <v>0</v>
       </c>
       <c r="H441" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I441" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J441" s="0" t="n">
         <v>0</v>
@@ -43496,10 +43502,10 @@
         <v>0</v>
       </c>
       <c r="H442" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I442" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J442" s="0" t="n">
         <v>0</v>
@@ -43516,10 +43522,10 @@
         <v>0</v>
       </c>
       <c r="H443" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I443" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J443" s="0" t="n">
         <v>0</v>
@@ -43536,10 +43542,10 @@
         <v>0</v>
       </c>
       <c r="H444" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I444" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J444" s="0" t="n">
         <v>0</v>
@@ -43559,10 +43565,10 @@
         <v>0</v>
       </c>
       <c r="H445" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I445" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J445" s="0" t="n">
         <v>0</v>
@@ -43582,10 +43588,10 @@
         <v>0</v>
       </c>
       <c r="H446" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I446" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J446" s="0" t="n">
         <v>0</v>
@@ -43602,10 +43608,10 @@
         <v>0</v>
       </c>
       <c r="H447" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I447" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J447" s="0" t="n">
         <v>0</v>
@@ -43622,10 +43628,10 @@
         <v>0</v>
       </c>
       <c r="H448" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I448" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J448" s="0" t="n">
         <v>0</v>
@@ -43642,10 +43648,10 @@
         <v>0</v>
       </c>
       <c r="H449" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I449" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J449" s="0" t="n">
         <v>0</v>
@@ -43662,10 +43668,10 @@
         <v>0</v>
       </c>
       <c r="H450" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I450" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J450" s="0" t="n">
         <v>0</v>
@@ -43682,10 +43688,10 @@
         <v>0</v>
       </c>
       <c r="H451" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I451" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J451" s="0" t="n">
         <v>0</v>
@@ -43705,10 +43711,10 @@
         <v>0</v>
       </c>
       <c r="H452" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I452" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J452" s="0" t="n">
         <v>0</v>
@@ -43725,10 +43731,10 @@
         <v>0</v>
       </c>
       <c r="H453" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I453" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J453" s="0" t="n">
         <v>0</v>
@@ -43745,10 +43751,10 @@
         <v>0</v>
       </c>
       <c r="H454" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I454" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J454" s="0" t="n">
         <v>0</v>
@@ -43765,10 +43771,10 @@
         <v>0</v>
       </c>
       <c r="H455" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I455" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J455" s="0" t="n">
         <v>0</v>
@@ -43785,10 +43791,10 @@
         <v>0</v>
       </c>
       <c r="H456" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I456" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J456" s="0" t="n">
         <v>0</v>
@@ -43805,10 +43811,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I457" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J457" s="0" t="n">
         <v>0</v>
@@ -43828,10 +43834,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I458" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J458" s="0" t="n">
         <v>0</v>
@@ -43851,10 +43857,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I459" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J459" s="0" t="n">
         <v>0</v>
@@ -43871,10 +43877,10 @@
         <v>0</v>
       </c>
       <c r="H460" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I460" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J460" s="0" t="n">
         <v>0</v>
@@ -43891,10 +43897,10 @@
         <v>0</v>
       </c>
       <c r="H461" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I461" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J461" s="0" t="n">
         <v>0</v>
@@ -43911,10 +43917,10 @@
         <v>0</v>
       </c>
       <c r="H462" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I462" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J462" s="0" t="n">
         <v>0</v>
@@ -43934,10 +43940,10 @@
         <v>0</v>
       </c>
       <c r="H463" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I463" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J463" s="0" t="n">
         <v>0</v>
@@ -43954,10 +43960,10 @@
         <v>0</v>
       </c>
       <c r="H464" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I464" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J464" s="0" t="n">
         <v>0</v>
@@ -43974,10 +43980,10 @@
         <v>0</v>
       </c>
       <c r="H465" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I465" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J465" s="0" t="n">
         <v>0</v>
@@ -43994,10 +44000,10 @@
         <v>0</v>
       </c>
       <c r="H466" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I466" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J466" s="0" t="n">
         <v>0</v>
@@ -44014,10 +44020,10 @@
         <v>0</v>
       </c>
       <c r="H467" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I467" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J467" s="0" t="n">
         <v>0</v>
@@ -44034,10 +44040,10 @@
         <v>0</v>
       </c>
       <c r="H468" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I468" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J468" s="0" t="n">
         <v>0</v>
@@ -44054,10 +44060,10 @@
         <v>0</v>
       </c>
       <c r="H469" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I469" s="0" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="J469" s="0" t="n">
         <v>0</v>

</xml_diff>